<commit_message>
Gammel Tidsregistereing der aldrig blev pushet
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Dan Toft.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Dan Toft.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -253,6 +253,30 @@
   </si>
   <si>
     <t>Review/bugfixes</t>
+  </si>
+  <si>
+    <t>Guikode</t>
+  </si>
+  <si>
+    <t>Det kan jeg ikke huske…</t>
+  </si>
+  <si>
+    <t>design oc5</t>
+  </si>
+  <si>
+    <t>Review OC11</t>
+  </si>
+  <si>
+    <t>Testsuite oc9</t>
+  </si>
+  <si>
+    <t>design review</t>
+  </si>
+  <si>
+    <t>Implamenter et eller andet</t>
+  </si>
+  <si>
+    <t>Review af design på OC13</t>
   </si>
 </sst>
 </file>
@@ -951,7 +975,7 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,154 +1503,185 @@
       <c r="C26" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="E26" s="10">
         <f t="shared" si="0"/>
         <v>0.33680555555555558</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="10">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G26" s="12">
         <f t="shared" si="3"/>
-        <v>-8.0833333333333339</v>
+        <v>7.416666666666667</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42811</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="10"/>
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G27" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.416666666666667</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
-        <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42814</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="E28" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="10"/>
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="G28" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.4166666666666656</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42814</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="10"/>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0.40277777777777773</v>
+      </c>
       <c r="G29" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.16666666666666607</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42814</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="9"/>
+      <c r="D30" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="E30" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="10"/>
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.51736111111111105</v>
+      </c>
       <c r="G30" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.7499999999999996</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42814</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="9"/>
+      <c r="D31" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="10"/>
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G31" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.5833333333333357</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42814</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="9"/>
+      <c r="D32" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="10"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G32" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="9"/>
+      <c r="D33" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="E33" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="10"/>
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0.375</v>
+      </c>
       <c r="G33" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.91666666666666607</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>49</v>
@@ -1634,18 +1689,18 @@
       <c r="D34" s="9"/>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>49</v>
@@ -1664,7 +1719,7 @@
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>49</v>
@@ -1683,7 +1738,7 @@
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>49</v>
@@ -1702,7 +1757,7 @@
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>49</v>
@@ -1721,7 +1776,7 @@
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>49</v>
@@ -1740,7 +1795,7 @@
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>49</v>
@@ -1759,7 +1814,7 @@
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>49</v>
@@ -1778,7 +1833,7 @@
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>49</v>
@@ -1797,7 +1852,7 @@
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>49</v>
@@ -1816,7 +1871,7 @@
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>49</v>
@@ -1835,7 +1890,7 @@
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>49</v>
@@ -1854,7 +1909,7 @@
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
         <f t="shared" si="1"/>
-        <v>42810</v>
+        <v>42815</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Über vigtigt tidsregistrering for ting jeg totalt meget ikke har glemt!
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Dan Toft.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Dan Toft.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,7 +21,7 @@
     <definedName name="Deltagere">Deltagere!$A$1:$A$16</definedName>
     <definedName name="GyldigeRoller">'Gyldige roller'!$A$1:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>Review af design på OC13</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Alt andet end gui og alligevel endte jeg med at lave GUI</t>
+  </si>
+  <si>
+    <t>Bugfixing</t>
   </si>
 </sst>
 </file>
@@ -974,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,78 +1695,94 @@
       <c r="C34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="9"/>
+      <c r="D34" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-      <c r="F34" s="10"/>
+      <c r="F34" s="10">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G34" s="12">
         <f t="shared" si="3"/>
-        <v>-9</v>
+        <v>6.5000000000000009</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42816</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="16"/>
+      <c r="D35" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="E35" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="17"/>
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F35" s="17">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G35" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.416666666666667</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42817</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="9"/>
+      <c r="D36" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="E36" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="10"/>
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F36" s="10">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G36" s="12">
         <f t="shared" ref="G36:G46" si="4">(F36-E36)*24</f>
-        <v>0</v>
+        <v>7.416666666666667</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="9"/>
+      <c r="D37" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="E37" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="10"/>
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G37" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.916666666666667</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>49</v>
@@ -1765,18 +1790,18 @@
       <c r="D38" s="9"/>
       <c r="E38" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>49</v>
@@ -1795,7 +1820,7 @@
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>49</v>
@@ -1814,7 +1839,7 @@
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>49</v>
@@ -1833,7 +1858,7 @@
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>49</v>
@@ -1852,7 +1877,7 @@
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>49</v>
@@ -1871,7 +1896,7 @@
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>49</v>
@@ -1890,7 +1915,7 @@
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>49</v>
@@ -1909,7 +1934,7 @@
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
         <f t="shared" si="1"/>
-        <v>42815</v>
+        <v>42818</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>49</v>

</xml_diff>